<commit_message>
FUNCTIONALITY: Finished testing the suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Testing")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -596,7 +596,7 @@
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
@@ -642,7 +642,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Finished automating the suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Step2Fields</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -531,7 +528,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +565,7 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Testing")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -596,7 +593,7 @@
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -604,13 +601,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -633,7 +630,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -642,7 +639,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,7 +648,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Removed a duplicate test case.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step2/_Test_Suite_Statistics.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,10 +617,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>